<commit_message>
update result 20201124 & update plan 20201125
</commit_message>
<xml_diff>
--- a/20201124.xlsx
+++ b/20201124.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swan3\Desktop\plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E1F664E-3FF4-4A5B-8581-CC9C6773E68F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CC796A0-81CE-42D3-8D6C-C5D0172C17C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-120" windowWidth="23256" windowHeight="12576" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="54">
   <si>
     <t>일</t>
   </si>
@@ -213,6 +213,33 @@
   </si>
   <si>
     <t>현대 미팅 (안할듯?)</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 피곤
+2. 피곤 
+3. 피곤 (월, 수, 금으로 변경)</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 어항 물 교체</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>피곤</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 모빌리티
+ - 2020.11.24 미팅 (현대 강남)
+  -&gt; BMS DFU 진행하기로 (최대 2ea)
+   =&gt; 12월11일 한 그전에 피앤이에서 테스트 요
+   =&gt; H1전문에서 Dock ID부여 요청 (이수혁D -&gt; 강훈식S)
+  -&gt; 추가 보완사항 (시연 중 발견)
+   =&gt; d1이 현재 오류상황에 여러 번 전송됨
+   =&gt; 시연 중 Ctid에 쓰레기 값이 검색되면서 동작 제대로 하지 않음
+   =&gt; LAN단선 및 485단선 후 재연결 시 e1전문이 날아가야 함
+   =&gt; DHCP관련 내용 먼저 수정 (지속적으로 DHCP요청 하도록)</t>
     <phoneticPr fontId="21" type="noConversion"/>
   </si>
 </sst>
@@ -386,7 +413,7 @@
       <charset val="129"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="41">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -600,6 +627,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -869,7 +920,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -900,28 +951,34 @@
     <xf numFmtId="0" fontId="1" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="38" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="39" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="39" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="40" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="40" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="38" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="1" fillId="32" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -933,23 +990,20 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="38" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="38" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="176" fontId="1" fillId="38" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -1538,16 +1592,20 @@
       </c>
     </row>
     <row r="3" spans="2:13" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="23"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="15" t="s">
+      <c r="D3" s="25"/>
+      <c r="E3" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="G3" s="18" t="s">
         <v>46</v>
       </c>
       <c r="H3" s="8"/>
@@ -1562,12 +1620,12 @@
       </c>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B4" s="20"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="15"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="18"/>
       <c r="H4" s="8"/>
       <c r="I4" t="s">
         <v>11</v>
@@ -1577,12 +1635,12 @@
       </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B5" s="20"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="15"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="18"/>
       <c r="H5" s="8"/>
       <c r="I5" t="s">
         <v>12</v>
@@ -1592,12 +1650,12 @@
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B6" s="20"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="15"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="18"/>
       <c r="H6" s="8"/>
       <c r="I6" t="s">
         <v>10</v>
@@ -1607,12 +1665,12 @@
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B7" s="20"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="15"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="18"/>
       <c r="H7" s="8"/>
       <c r="I7" t="s">
         <v>8</v>
@@ -1626,12 +1684,12 @@
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B8" s="20"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="15"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="18"/>
       <c r="H8" s="8"/>
       <c r="I8" t="s">
         <v>4</v>
@@ -1644,195 +1702,201 @@
       <c r="B9" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="15"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="18"/>
       <c r="H9" s="8"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B10" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="15"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="18"/>
       <c r="H10" s="8"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B11" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="D11" s="10"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="15"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="18"/>
       <c r="H11" s="8"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B12" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="13"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="15"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="18"/>
       <c r="H12" s="8"/>
     </row>
     <row r="13" spans="2:13" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="15"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="18"/>
       <c r="H13" s="8"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B14" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D14" s="13"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="15"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="18"/>
       <c r="H14" s="8"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="10"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="16"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="18" t="s">
+        <v>50</v>
+      </c>
       <c r="H15" s="8"/>
     </row>
     <row r="16" spans="2:13" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="13"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="17"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="19"/>
       <c r="H16" s="8"/>
     </row>
     <row r="17" spans="2:8" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="D17" s="10"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="17"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="19"/>
       <c r="H17" s="8"/>
     </row>
     <row r="18" spans="2:8" ht="33" x14ac:dyDescent="0.3">
       <c r="B18" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="26" t="s">
+      <c r="C18" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="D18" s="13"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="17"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="19"/>
       <c r="H18" s="8"/>
     </row>
     <row r="19" spans="2:8" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="10"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="17"/>
+      <c r="D19" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="E19" s="20"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="19"/>
       <c r="H19" s="8"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B20" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="D20" s="14"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="25"/>
-      <c r="G20" s="17"/>
+      <c r="D20" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="E20" s="20"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="19"/>
       <c r="H20" s="8"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B21" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="D21" s="10"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="17"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="19"/>
       <c r="H21" s="8"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B22" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="D22" s="13"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="25"/>
-      <c r="G22" s="17"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="19"/>
       <c r="H22" s="8"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B23" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D23" s="12"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="25"/>
-      <c r="G23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="19"/>
       <c r="H23" s="8"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.3">

</xml_diff>